<commit_message>
Cast Charge 21 - C11. Almost out of Zn for future castings
</commit_message>
<xml_diff>
--- a/Charge 20 - C10.xlsx
+++ b/Charge 20 - C10.xlsx
@@ -4920,7 +4920,7 @@
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="173" t="str">
         <f>"Actual  " &amp; 'Charge 20'!I3</f>
-        <v>Actual  Mg0Ca100</v>
+        <v>Actual  Mg65Zn30Ca5</v>
       </c>
       <c r="B3" s="174"/>
       <c r="C3" s="174"/>
@@ -4982,17 +4982,17 @@
       <c r="A6" s="26">
         <v>1</v>
       </c>
-      <c r="B6" s="105" t="str">
+      <c r="B6" s="105">
         <f>IF('Charge 20'!B14=0, "-", 'Charge 20'!B14)</f>
-        <v>-</v>
-      </c>
-      <c r="C6" s="137" t="str">
+        <v>6.8170000000000002</v>
+      </c>
+      <c r="C6" s="137">
         <f>IF('Charge 20'!E14=0,"-",'Charge 20'!E14)</f>
-        <v>-</v>
+        <v>11.855</v>
       </c>
       <c r="D6" s="137">
         <f>IF('Charge 20'!H14=0, "-", 'Charge 20'!H14)</f>
-        <v>5.327</v>
+        <v>5.2549999999999999</v>
       </c>
       <c r="E6" s="137" t="str">
         <f>IF('Charge 20'!K14=0, "-", 'Charge 20'!K14)</f>
@@ -5004,7 +5004,7 @@
       </c>
       <c r="G6" s="138">
         <f>COUNTIF(B6:B20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H6" s="131" t="str">
         <f>B4</f>
@@ -5015,13 +5015,13 @@
       <c r="A7" s="27">
         <v>2</v>
       </c>
-      <c r="B7" s="108" t="str">
+      <c r="B7" s="108">
         <f>IF('Charge 20'!B15=0, "-", 'Charge 20'!B15)</f>
-        <v>-</v>
-      </c>
-      <c r="C7" s="107" t="str">
+        <v>7.6779999999999999</v>
+      </c>
+      <c r="C7" s="107">
         <f>IF('Charge 20'!E15=0,"-",'Charge 20'!E15)</f>
-        <v>-</v>
+        <v>16.52</v>
       </c>
       <c r="D7" s="107" t="str">
         <f>IF('Charge 20'!H15=0, "-", 'Charge 20'!H15)</f>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="G7" s="106">
         <f>COUNTIF(C6:C20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H7" s="151" t="str">
         <f>C4</f>
@@ -5048,13 +5048,13 @@
       <c r="A8" s="27">
         <v>3</v>
       </c>
-      <c r="B8" s="108" t="str">
+      <c r="B8" s="108">
         <f>IF('Charge 20'!B16=0, "-", 'Charge 20'!B16)</f>
-        <v>-</v>
-      </c>
-      <c r="C8" s="107" t="str">
+        <v>7.742</v>
+      </c>
+      <c r="C8" s="107">
         <f>IF('Charge 20'!E16=0,"-",'Charge 20'!E16)</f>
-        <v>-</v>
+        <v>23.068999999999999</v>
       </c>
       <c r="D8" s="107" t="str">
         <f>IF('Charge 20'!H16=0, "-", 'Charge 20'!H16)</f>
@@ -5081,9 +5081,9 @@
       <c r="A9" s="27">
         <v>4</v>
       </c>
-      <c r="B9" s="108" t="str">
+      <c r="B9" s="108">
         <f>IF('Charge 20'!B17=0, "-", 'Charge 20'!B17)</f>
-        <v>-</v>
+        <v>7.8520000000000003</v>
       </c>
       <c r="C9" s="107" t="str">
         <f>IF('Charge 20'!E17=0,"-",'Charge 20'!E17)</f>
@@ -5114,9 +5114,9 @@
       <c r="A10" s="27">
         <v>5</v>
       </c>
-      <c r="B10" s="108" t="str">
+      <c r="B10" s="108">
         <f>IF('Charge 20'!B18=0, "-", 'Charge 20'!B18)</f>
-        <v>-</v>
+        <v>11.343999999999999</v>
       </c>
       <c r="C10" s="107" t="str">
         <f>IF('Charge 20'!E18=0,"-",'Charge 20'!E18)</f>
@@ -5169,7 +5169,7 @@
       </c>
       <c r="G11" s="160">
         <f>COUNTIF(B6:F20, "&lt;&gt;-")</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H11" s="153" t="str">
         <f>G4</f>
@@ -5416,15 +5416,15 @@
       </c>
       <c r="B21" s="77">
         <f>SUM(B6:B20)</f>
-        <v>0</v>
+        <v>41.433</v>
       </c>
       <c r="C21" s="37">
         <f>SUM(C6:C20)</f>
-        <v>0</v>
+        <v>51.444000000000003</v>
       </c>
       <c r="D21" s="69">
         <f>SUM(D6:D20)</f>
-        <v>5.327</v>
+        <v>5.2549999999999999</v>
       </c>
       <c r="E21" s="69">
         <f>SUM(E6:E20)</f>
@@ -5436,7 +5436,7 @@
       </c>
       <c r="G21" s="144">
         <f>SUM(B21:F21)</f>
-        <v>5.327</v>
+        <v>98.132000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5445,15 +5445,15 @@
       </c>
       <c r="B22" s="145">
         <f>'Charge 20'!F4</f>
-        <v>42.116999999999997</v>
+        <v>41.430999999999997</v>
       </c>
       <c r="C22" s="135">
         <f>'Charge 20'!F5</f>
-        <v>52.290999999999997</v>
+        <v>51.439</v>
       </c>
       <c r="D22" s="135">
         <f>'Charge 20'!F6</f>
-        <v>5.3419999999999996</v>
+        <v>5.2549999999999999</v>
       </c>
       <c r="E22" s="135">
         <f>'Charge 20'!F7</f>
@@ -5465,7 +5465,7 @@
       </c>
       <c r="G22" s="70">
         <f>SUM(B22:F22)</f>
-        <v>99.749999999999986</v>
+        <v>98.125</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5474,15 +5474,15 @@
       </c>
       <c r="B23" s="146">
         <f>B21-B22</f>
-        <v>-42.116999999999997</v>
+        <v>2.0000000000024443E-3</v>
       </c>
       <c r="C23" s="140">
         <f t="shared" ref="C23:G23" si="0">C21-C22</f>
-        <v>-52.290999999999997</v>
+        <v>5.000000000002558E-3</v>
       </c>
       <c r="D23" s="140">
         <f t="shared" si="0"/>
-        <v>-1.499999999999968E-2</v>
+        <v>0</v>
       </c>
       <c r="E23" s="140">
         <f t="shared" si="0"/>
@@ -5494,7 +5494,7 @@
       </c>
       <c r="G23" s="113">
         <f t="shared" si="0"/>
-        <v>-94.422999999999988</v>
+        <v>7.0000000000050022E-3</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -5520,7 +5520,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G1"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="I3" s="62" t="str">
         <f>Q4 &amp; ROUND(N4,3)*100 &amp; IF(N5=0, "", Q5 &amp; ROUND(N5,3)*100) &amp; IF(N6=0, "", Q6 &amp; ROUND(N6,3)*100) &amp; IF(N7=0, "", Q7 &amp; ROUND(N7,3)*100) &amp; IF(N8=0, "", Q8 &amp; ROUND(N8,3)*100)</f>
-        <v>Mg0Ca100</v>
+        <v>Mg65Zn30Ca5</v>
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="s">
@@ -5683,11 +5683,11 @@
       </c>
       <c r="F4" s="69">
         <f>IF($F$9=0, ROUND($F$10*E4, 3), ROUND(E4*$F$9, 3))</f>
-        <v>42.116999999999997</v>
+        <v>41.430999999999997</v>
       </c>
       <c r="G4" s="70">
         <f>IFERROR(F4/U4, 0)</f>
-        <v>24.233026467203683</v>
+        <v>23.838319907940161</v>
       </c>
       <c r="I4" s="71" t="str">
         <f>$Q$4</f>
@@ -5696,19 +5696,19 @@
       <c r="J4" s="26"/>
       <c r="K4" s="72">
         <f>B29</f>
-        <v>0</v>
+        <v>41.433</v>
       </c>
       <c r="L4" s="73">
         <f>K4/$K$9</f>
-        <v>0</v>
+        <v>0.42221701381812249</v>
       </c>
       <c r="M4" s="23">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>0</v>
+        <v>1.7371611348204998E-2</v>
       </c>
       <c r="N4" s="115">
         <f>M4/$M$9</f>
-        <v>0</v>
+        <v>0.64999502095497785</v>
       </c>
       <c r="P4" s="15">
         <v>1</v>
@@ -5780,11 +5780,11 @@
       </c>
       <c r="F5" s="69">
         <f t="shared" ref="F5:F8" si="0">IF($F$9=0, ROUND($F$10*E5, 3), ROUND(E5*$F$9, 3))</f>
-        <v>52.290999999999997</v>
+        <v>51.439</v>
       </c>
       <c r="G5" s="70">
         <f>IFERROR(F5/U5, 0)</f>
-        <v>7.3236694677871146</v>
+        <v>7.204341736694678</v>
       </c>
       <c r="I5" s="71" t="str">
         <f>$Q$5</f>
@@ -5793,19 +5793,19 @@
       <c r="J5" s="27"/>
       <c r="K5" s="75">
         <f>E29</f>
-        <v>0</v>
+        <v>51.444000000000003</v>
       </c>
       <c r="L5" s="76">
         <f>K5/$K$9</f>
-        <v>0</v>
+        <v>0.52423266620470388</v>
       </c>
       <c r="M5" s="24">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>0</v>
+        <v>8.0179967912377085E-3</v>
       </c>
       <c r="N5" s="116">
         <f>M5/$M$9</f>
-        <v>0</v>
+        <v>0.30001005018316956</v>
       </c>
       <c r="P5" s="15">
         <v>2</v>
@@ -5877,11 +5877,11 @@
       </c>
       <c r="F6" s="69">
         <f t="shared" si="0"/>
-        <v>5.3419999999999996</v>
+        <v>5.2549999999999999</v>
       </c>
       <c r="G6" s="70">
         <f>IFERROR(F6/U6, 0)</f>
-        <v>3.4464516129032257</v>
+        <v>3.3903225806451611</v>
       </c>
       <c r="I6" s="71" t="str">
         <f>$Q$6</f>
@@ -5890,19 +5890,19 @@
       <c r="J6" s="27"/>
       <c r="K6" s="77">
         <f>H29</f>
-        <v>5.327</v>
+        <v>5.2549999999999999</v>
       </c>
       <c r="L6" s="76">
         <f>K6/$K$9</f>
-        <v>1</v>
+        <v>5.3550319977173598E-2</v>
       </c>
       <c r="M6" s="24">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>2.4951344877488894E-2</v>
+        <v>1.3361525020503416E-3</v>
       </c>
       <c r="N6" s="116">
         <f>M6/$M$9</f>
-        <v>1</v>
+        <v>4.9994928861852465E-2</v>
       </c>
       <c r="P6" s="15">
         <v>3</v>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="G9" s="144">
         <f>SUM(G4:G8)</f>
-        <v>35.003147547894024</v>
+        <v>34.432984225280002</v>
       </c>
       <c r="I9" s="82"/>
       <c r="J9" s="79" t="s">
@@ -6178,7 +6178,7 @@
       </c>
       <c r="K9" s="117">
         <f>SUM(K4:K8)</f>
-        <v>5.327</v>
+        <v>98.132000000000005</v>
       </c>
       <c r="L9" s="83">
         <f>SUM(L4:L8)</f>
@@ -6186,11 +6186,11 @@
       </c>
       <c r="M9" s="118">
         <f>SUM(M4:M8)</f>
-        <v>2.4951344877488894E-2</v>
+        <v>2.6725760641493051E-2</v>
       </c>
       <c r="N9" s="84">
         <f>SUM(N4:N8)</f>
-        <v>1</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>111</v>
@@ -6232,10 +6232,10 @@
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F10" s="158">
         <f>G10*U9</f>
-        <v>99.75</v>
+        <v>98.125500000000002</v>
       </c>
       <c r="G10" s="9">
-        <v>35</v>
+        <v>34.43</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="26.25" x14ac:dyDescent="0.4">
@@ -6341,7 +6341,7 @@
       </c>
       <c r="B14" s="106">
         <f>A!C2</f>
-        <v>0</v>
+        <v>6.8170000000000002</v>
       </c>
       <c r="C14" s="107"/>
       <c r="D14" s="126">
@@ -6349,7 +6349,7 @@
       </c>
       <c r="E14" s="106">
         <f>B!C2</f>
-        <v>0</v>
+        <v>11.855</v>
       </c>
       <c r="F14" s="107"/>
       <c r="G14" s="126">
@@ -6357,7 +6357,7 @@
       </c>
       <c r="H14" s="106">
         <f>'C'!C2</f>
-        <v>5.327</v>
+        <v>5.2549999999999999</v>
       </c>
       <c r="I14" s="107"/>
       <c r="J14" s="126">
@@ -6394,7 +6394,7 @@
       </c>
       <c r="B15" s="106">
         <f>A!C3</f>
-        <v>0</v>
+        <v>7.6779999999999999</v>
       </c>
       <c r="C15" s="107"/>
       <c r="D15" s="126">
@@ -6402,7 +6402,7 @@
       </c>
       <c r="E15" s="106">
         <f>B!C3</f>
-        <v>0</v>
+        <v>16.52</v>
       </c>
       <c r="F15" s="107"/>
       <c r="G15" s="126">
@@ -6447,7 +6447,7 @@
       </c>
       <c r="B16" s="106">
         <f>A!C4</f>
-        <v>0</v>
+        <v>7.742</v>
       </c>
       <c r="C16" s="107"/>
       <c r="D16" s="126">
@@ -6455,7 +6455,7 @@
       </c>
       <c r="E16" s="106">
         <f>B!C4</f>
-        <v>0</v>
+        <v>23.068999999999999</v>
       </c>
       <c r="F16" s="107"/>
       <c r="G16" s="126">
@@ -6500,7 +6500,7 @@
       </c>
       <c r="B17" s="106">
         <f>A!C5</f>
-        <v>0</v>
+        <v>7.8520000000000003</v>
       </c>
       <c r="C17" s="107"/>
       <c r="D17" s="126">
@@ -6553,7 +6553,7 @@
       </c>
       <c r="B18" s="106">
         <f>A!C6</f>
-        <v>0</v>
+        <v>11.343999999999999</v>
       </c>
       <c r="C18" s="107"/>
       <c r="D18" s="126">
@@ -7059,7 +7059,7 @@
       </c>
       <c r="B29" s="110">
         <f>SUM(B14:B28)</f>
-        <v>0</v>
+        <v>41.433</v>
       </c>
       <c r="C29" s="107"/>
       <c r="D29" s="109" t="s">
@@ -7067,7 +7067,7 @@
       </c>
       <c r="E29" s="111">
         <f>SUM(E14:E28)</f>
-        <v>0</v>
+        <v>51.444000000000003</v>
       </c>
       <c r="F29" s="107"/>
       <c r="G29" s="109" t="s">
@@ -7075,7 +7075,7 @@
       </c>
       <c r="H29" s="110">
         <f>SUM(H14:H28)</f>
-        <v>5.327</v>
+        <v>5.2549999999999999</v>
       </c>
       <c r="I29" s="107"/>
       <c r="J29" s="109" t="s">
@@ -7100,7 +7100,7 @@
       </c>
       <c r="B30" s="113">
         <f>B29-$F$4</f>
-        <v>-42.116999999999997</v>
+        <v>2.0000000000024443E-3</v>
       </c>
       <c r="C30" s="114"/>
       <c r="D30" s="112" t="s">
@@ -7108,7 +7108,7 @@
       </c>
       <c r="E30" s="113">
         <f>E29-$F$5</f>
-        <v>-52.290999999999997</v>
+        <v>5.000000000002558E-3</v>
       </c>
       <c r="F30" s="114"/>
       <c r="G30" s="112" t="s">
@@ -7116,7 +7116,7 @@
       </c>
       <c r="H30" s="113">
         <f>H29-$F$6</f>
-        <v>-1.499999999999968E-2</v>
+        <v>0</v>
       </c>
       <c r="I30" s="114"/>
       <c r="J30" s="112" t="s">
@@ -8522,7 +8522,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -8557,37 +8557,37 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="166">
-        <v>5.4939999999999998</v>
+        <v>6.8170000000000002</v>
       </c>
       <c r="B2" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <f>IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
+        <v>6.8170000000000002</v>
       </c>
       <c r="D2" s="1">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>41.433</v>
       </c>
       <c r="E2" s="127" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="129">
         <f>'Charge 20'!F4</f>
-        <v>42.116999999999997</v>
+        <v>41.430999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="166">
-        <v>5.5179999999999998</v>
+        <v>7.6779999999999999</v>
       </c>
       <c r="B3" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f>IF(A3=0, 0, A3*B3)</f>
-        <v>0</v>
+        <v>7.6779999999999999</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="127" t="s">
@@ -8595,19 +8595,19 @@
       </c>
       <c r="F3" s="129">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>41.433</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="166">
-        <v>5.5990000000000002</v>
+        <v>7.742</v>
       </c>
       <c r="B4" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <f>IF(A4=0, 0, A4*B4)</f>
-        <v>0</v>
+        <v>7.742</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="127" t="s">
@@ -8615,37 +8615,37 @@
       </c>
       <c r="F4" s="129">
         <f>F3-F2</f>
-        <v>-42.116999999999997</v>
+        <v>2.0000000000024443E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="166">
-        <v>5.8650000000000002</v>
+        <v>7.8520000000000003</v>
       </c>
       <c r="B5" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f>IF(A5=0, 0, A5*B5)</f>
-        <v>0</v>
+        <v>7.8520000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="166">
-        <v>6.1580000000000004</v>
+        <v>11.343999999999999</v>
       </c>
       <c r="B6" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f>IF(A6=0, 0, A6*B6)</f>
-        <v>0</v>
+        <v>11.343999999999999</v>
       </c>
       <c r="E6" s="167"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="166">
-        <v>6.3570000000000002</v>
+        <v>4.4889999999999999</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
@@ -8657,7 +8657,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="166">
-        <v>7.6779999999999999</v>
+        <v>4.7530000000000001</v>
       </c>
       <c r="B8" s="125">
         <v>0</v>
@@ -8670,7 +8670,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="166">
-        <v>11.292</v>
+        <v>4.9779999999999998</v>
       </c>
       <c r="B9" s="125">
         <v>0</v>
@@ -8681,7 +8681,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="166"/>
+      <c r="A10" s="166">
+        <v>5.1539999999999999</v>
+      </c>
       <c r="B10" s="125">
         <v>0</v>
       </c>
@@ -8691,7 +8693,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="166"/>
+      <c r="A11" s="166">
+        <v>5.1539999999999999</v>
+      </c>
       <c r="B11" s="125">
         <v>0</v>
       </c>
@@ -8701,7 +8705,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="166"/>
+      <c r="A12" s="166">
+        <v>5.3550000000000004</v>
+      </c>
       <c r="B12" s="125">
         <v>0</v>
       </c>
@@ -8711,7 +8717,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="166"/>
+      <c r="A13" s="166">
+        <v>5.4939999999999998</v>
+      </c>
       <c r="B13" s="125">
         <v>0</v>
       </c>
@@ -8721,7 +8729,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="166"/>
+      <c r="A14" s="166">
+        <v>5.5179999999999998</v>
+      </c>
       <c r="B14" s="125">
         <v>0</v>
       </c>
@@ -8731,7 +8741,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="166"/>
+      <c r="A15" s="166">
+        <v>5.5990000000000002</v>
+      </c>
       <c r="B15" s="125">
         <v>0</v>
       </c>
@@ -8741,7 +8753,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="166"/>
+      <c r="A16" s="166">
+        <v>5.6849999999999996</v>
+      </c>
       <c r="B16" s="125">
         <v>0</v>
       </c>
@@ -8751,7 +8765,9 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="166"/>
+      <c r="A17" s="166">
+        <v>5.8220000000000001</v>
+      </c>
       <c r="B17" s="125">
         <v>0</v>
       </c>
@@ -8761,7 +8777,9 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="166"/>
+      <c r="A18" s="166">
+        <v>5.8650000000000002</v>
+      </c>
       <c r="B18" s="125">
         <v>0</v>
       </c>
@@ -8771,7 +8789,9 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="166"/>
+      <c r="A19" s="166">
+        <v>5.8879999999999999</v>
+      </c>
       <c r="B19" s="125">
         <v>0</v>
       </c>
@@ -8781,7 +8801,9 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="166"/>
+      <c r="A20" s="166">
+        <v>6.1580000000000004</v>
+      </c>
       <c r="B20" s="125">
         <v>0</v>
       </c>
@@ -8791,7 +8813,9 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="166"/>
+      <c r="A21" s="166">
+        <v>6.343</v>
+      </c>
       <c r="B21" s="125">
         <v>0</v>
       </c>
@@ -8801,7 +8825,9 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="166"/>
+      <c r="A22" s="166">
+        <v>6.3570000000000002</v>
+      </c>
       <c r="B22" s="125">
         <v>0</v>
       </c>
@@ -8811,7 +8837,9 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="166"/>
+      <c r="A23" s="166">
+        <v>6.4370000000000003</v>
+      </c>
       <c r="B23" s="125">
         <v>0</v>
       </c>
@@ -8821,7 +8849,9 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="166"/>
+      <c r="A24" s="166">
+        <v>7.89</v>
+      </c>
       <c r="B24" s="125">
         <v>0</v>
       </c>
@@ -8831,7 +8861,9 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="166"/>
+      <c r="A25" s="166">
+        <v>8.9039999999999999</v>
+      </c>
       <c r="B25" s="125">
         <v>0</v>
       </c>
@@ -8841,7 +8873,9 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="166"/>
+      <c r="A26" s="166">
+        <v>9.7080000000000002</v>
+      </c>
       <c r="B26" s="125">
         <v>0</v>
       </c>
@@ -8851,7 +8885,9 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="166"/>
+      <c r="A27" s="166">
+        <v>10.33</v>
+      </c>
       <c r="B27" s="125">
         <v>0</v>
       </c>
@@ -8861,7 +8897,9 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="166"/>
+      <c r="A28" s="166">
+        <v>10.664</v>
+      </c>
       <c r="B28" s="125">
         <v>0</v>
       </c>
@@ -8871,7 +8909,9 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="166"/>
+      <c r="A29" s="166">
+        <v>11.292</v>
+      </c>
       <c r="B29" s="125">
         <v>0</v>
       </c>
@@ -8881,7 +8921,9 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="166"/>
+      <c r="A30" s="166">
+        <v>11.41</v>
+      </c>
       <c r="B30" s="125">
         <v>0</v>
       </c>
@@ -8891,7 +8933,9 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="166"/>
+      <c r="A31" s="166">
+        <v>11.769</v>
+      </c>
       <c r="B31" s="125">
         <v>0</v>
       </c>
@@ -8901,7 +8945,9 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="166"/>
+      <c r="A32" s="166">
+        <v>12.035</v>
+      </c>
       <c r="B32" s="125">
         <v>0</v>
       </c>
@@ -8911,7 +8957,9 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="166"/>
+      <c r="A33" s="166">
+        <v>12.468999999999999</v>
+      </c>
       <c r="B33" s="125">
         <v>0</v>
       </c>
@@ -8921,7 +8969,9 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="166"/>
+      <c r="A34" s="166">
+        <v>13.587999999999999</v>
+      </c>
       <c r="B34" s="125">
         <v>0</v>
       </c>
@@ -9103,7 +9153,7 @@
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition ref="A1"/>
+      <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9120,7 +9170,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -9158,22 +9208,22 @@
         <v>11.855</v>
       </c>
       <c r="B2" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <f>IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
+        <v>11.855</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>51.444000000000003</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="51">
         <f>'Charge 20'!F5</f>
-        <v>52.290999999999997</v>
+        <v>51.439</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9181,84 +9231,84 @@
         <v>16.52</v>
       </c>
       <c r="B3" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <f>IF(A3=0, 0, A3*B3)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>16.52</v>
       </c>
       <c r="E3" s="50" t="s">
         <v>105</v>
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>51.444000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="125">
-        <v>17.268000000000001</v>
+        <v>23.068999999999999</v>
       </c>
       <c r="B4" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <f>IF(A4=0, 0, A4*B4)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>23.068999999999999</v>
       </c>
       <c r="E4" s="50" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="51">
         <f>F3-F2</f>
-        <v>-52.290999999999997</v>
+        <v>5.000000000002558E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="125">
-        <v>18.271999999999998</v>
+        <v>17.268000000000001</v>
       </c>
       <c r="B5" s="125">
         <v>0</v>
       </c>
       <c r="C5">
-        <f>IF(A5=0, 0, A5*B5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="125">
-        <v>20.597000000000001</v>
+        <v>18.271999999999998</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IF(A6=0, 0, A6*B6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="125">
-        <v>21.074999999999999</v>
+        <v>20.597000000000001</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
       </c>
       <c r="C7">
-        <f>IF(A7=0, 0, A7*B7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="125">
-        <v>23.068999999999999</v>
+        <v>21.074999999999999</v>
       </c>
       <c r="B8" s="125">
         <v>0</v>
       </c>
       <c r="C8">
-        <f>IF(A8=0, 0, A8*B8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9270,7 +9320,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IF(A9=0, 0, A9*B9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9280,7 +9330,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(A10=0, 0, A10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9290,7 +9340,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(A11=0, 0, A11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9300,7 +9350,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(A12=0, 0, A12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9310,7 +9360,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(A13=0, 0, A13*B13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9320,7 +9370,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IF(A14=0, 0, A14*B14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9330,7 +9380,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IF(A15=0, 0, A15*B15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9340,7 +9390,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IF(A16=0, 0, A16*B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9350,7 +9400,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>IF(A17=0, 0, A17*B17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9360,7 +9410,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>IF(A18=0, 0, A18*B18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9370,7 +9420,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>IF(A19=0, 0, A19*B19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9380,7 +9430,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>IF(A20=0, 0, A20*B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9390,7 +9440,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f>IF(A21=0, 0, A21*B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9400,7 +9450,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>IF(A22=0, 0, A22*B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9410,7 +9460,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>IF(A23=0, 0, A23*B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9420,7 +9470,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>IF(A24=0, 0, A24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9430,7 +9480,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>IF(A25=0, 0, A25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9440,7 +9490,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f>IF(A26=0, 0, A26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9450,7 +9500,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f>IF(A27=0, 0, A27*B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9460,7 +9510,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>IF(A28=0, 0, A28*B28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9470,7 +9520,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f>IF(A29=0, 0, A29*B29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9480,7 +9530,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f>IF(A30=0, 0, A30*B30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9490,7 +9540,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f>IF(A31=0, 0, A31*B31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9500,7 +9550,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f>IF(A32=0, 0, A32*B32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9510,7 +9560,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>IF(A33=0, 0, A33*B33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9520,7 +9570,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f>IF(A34=0, 0, A34*B34)</f>
+        <f t="shared" ref="C34:C65" si="1">IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -9530,7 +9580,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f>IF(A35=0, 0, A35*B35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9540,7 +9590,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f>IF(A36=0, 0, A36*B36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9550,7 +9600,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f>IF(A37=0, 0, A37*B37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9560,7 +9610,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f>IF(A38=0, 0, A38*B38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9570,7 +9620,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f>IF(A39=0, 0, A39*B39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9580,7 +9630,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f>IF(A40=0, 0, A40*B40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9590,7 +9640,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f>IF(A41=0, 0, A41*B41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9600,7 +9650,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f>IF(A42=0, 0, A42*B42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9610,7 +9660,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f>IF(A43=0, 0, A43*B43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9620,7 +9670,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f>IF(A44=0, 0, A44*B44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9630,7 +9680,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f>IF(A45=0, 0, A45*B45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9640,7 +9690,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f>IF(A46=0, 0, A46*B46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9650,7 +9700,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f>IF(A47=0, 0, A47*B47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9660,7 +9710,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f>IF(A48=0, 0, A48*B48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9670,7 +9720,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f>IF(A49=0, 0, A49*B49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9680,7 +9730,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f>IF(A50=0, 0, A50*B50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9690,14 +9740,14 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f>IF(A51=0, 0, A51*B51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition ref="A1"/>
+      <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9749,25 +9799,25 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>5.327</v>
+        <v>5.2549999999999999</v>
       </c>
       <c r="B2" s="125">
         <v>1</v>
       </c>
       <c r="C2">
         <f>IF(A2=0, 0, A2*B2)</f>
-        <v>5.327</v>
+        <v>5.2549999999999999</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>5.327</v>
+        <v>5.2549999999999999</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="51">
         <f>'Charge 20'!F6</f>
-        <v>5.3419999999999996</v>
+        <v>5.2549999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9784,7 +9834,7 @@
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>5.327</v>
+        <v>5.2549999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9801,7 +9851,7 @@
       </c>
       <c r="F4" s="51">
         <f>F3-F2</f>
-        <v>-1.499999999999968E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>